<commit_message>
Fixed some bugs, added Unsafe Mode
</commit_message>
<xml_diff>
--- a/scripts/MHW Layered Armor.xlsx
+++ b/scripts/MHW Layered Armor.xlsx
@@ -1461,7 +1461,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1478,12 +1478,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1521,7 +1515,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1547,10 +1541,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1589,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:M256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A198" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G209" activeCellId="0" sqref="G209"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G239" activeCellId="0" sqref="G239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6040,23 +6030,23 @@
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
     </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B165" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="C165" s="7" t="s">
+      <c r="C165" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="D165" s="7" t="s">
+      <c r="D165" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="E165" s="7" t="s">
+      <c r="E165" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="F165" s="7" t="s">
+      <c r="F165" s="0" t="s">
         <v>320</v>
       </c>
       <c r="G165" s="1"/>
@@ -6067,23 +6057,23 @@
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B166" s="7" t="s">
+      <c r="B166" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="C166" s="7" t="s">
+      <c r="C166" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="D166" s="7" t="s">
+      <c r="D166" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="E166" s="7" t="s">
+      <c r="E166" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="F166" s="7" t="s">
+      <c r="F166" s="0" t="s">
         <v>322</v>
       </c>
       <c r="G166" s="1"/>
@@ -6094,23 +6084,23 @@
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
     </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B167" s="7" t="s">
+      <c r="B167" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="C167" s="7" t="s">
+      <c r="C167" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="D167" s="7" t="s">
+      <c r="D167" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="E167" s="7" t="s">
+      <c r="E167" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="F167" s="7" t="s">
+      <c r="F167" s="0" t="s">
         <v>324</v>
       </c>
       <c r="G167" s="1"/>
@@ -6776,16 +6766,16 @@
       <c r="B192" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C192" s="8" t="s">
+      <c r="C192" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="D192" s="8" t="s">
+      <c r="D192" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="E192" s="8" t="s">
+      <c r="E192" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="F192" s="8" t="s">
+      <c r="F192" s="7" t="s">
         <v>359</v>
       </c>
       <c r="G192" s="1"/>
@@ -6803,16 +6793,16 @@
       <c r="B193" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C193" s="8" t="s">
+      <c r="C193" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="D193" s="8" t="s">
+      <c r="D193" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E193" s="8" t="s">
+      <c r="E193" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="F193" s="8" t="s">
+      <c r="F193" s="7" t="s">
         <v>362</v>
       </c>
       <c r="G193" s="1"/>
@@ -6908,7 +6898,7 @@
       <c r="A197" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B197" s="9" t="s">
+      <c r="B197" s="8" t="s">
         <v>369</v>
       </c>
       <c r="C197" s="1" t="s">
@@ -7070,22 +7060,22 @@
       <c r="A203" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B203" s="10" t="s">
+      <c r="B203" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C203" s="10" t="s">
+      <c r="C203" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D203" s="10" t="s">
+      <c r="D203" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E203" s="10" t="s">
+      <c r="E203" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F203" s="10" t="s">
+      <c r="F203" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G203" s="10" t="s">
+      <c r="G203" s="9" t="s">
         <v>379</v>
       </c>
       <c r="H203" s="1"/>
@@ -7099,22 +7089,22 @@
       <c r="A204" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B204" s="10" t="s">
+      <c r="B204" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C204" s="10" t="s">
+      <c r="C204" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="D204" s="10" t="s">
+      <c r="D204" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="E204" s="10" t="s">
+      <c r="E204" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="F204" s="10" t="s">
+      <c r="F204" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="G204" s="10" t="s">
+      <c r="G204" s="9" t="s">
         <v>379</v>
       </c>
       <c r="H204" s="1"/>
@@ -7128,25 +7118,25 @@
       <c r="A205" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B205" s="10" t="s">
+      <c r="B205" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="C205" s="10" t="s">
+      <c r="C205" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D205" s="10" t="s">
+      <c r="D205" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E205" s="10" t="s">
+      <c r="E205" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="F205" s="10" t="s">
+      <c r="F205" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="G205" s="10" t="s">
+      <c r="G205" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="H205" s="11"/>
+      <c r="H205" s="10"/>
       <c r="I205" s="1"/>
       <c r="J205" s="1"/>
       <c r="K205" s="1"/>
@@ -7157,22 +7147,22 @@
       <c r="A206" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B206" s="10" t="s">
+      <c r="B206" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="C206" s="10" t="s">
+      <c r="C206" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="D206" s="10" t="s">
+      <c r="D206" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="E206" s="10" t="s">
+      <c r="E206" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="F206" s="10" t="s">
+      <c r="F206" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="G206" s="10" t="s">
+      <c r="G206" s="9" t="s">
         <v>384</v>
       </c>
       <c r="H206" s="1"/>
@@ -7186,22 +7176,22 @@
       <c r="A207" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="B207" s="10" t="s">
+      <c r="B207" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="C207" s="10" t="s">
+      <c r="C207" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="D207" s="10" t="s">
+      <c r="D207" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="E207" s="10" t="s">
+      <c r="E207" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="F207" s="10" t="s">
+      <c r="F207" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="G207" s="10" t="s">
+      <c r="G207" s="9" t="s">
         <v>384</v>
       </c>
       <c r="H207" s="1"/>
@@ -7215,22 +7205,22 @@
       <c r="A208" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B208" s="10" t="s">
+      <c r="B208" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C208" s="10" t="s">
+      <c r="C208" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="D208" s="10" t="s">
+      <c r="D208" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="E208" s="10" t="s">
+      <c r="E208" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="F208" s="10" t="s">
+      <c r="F208" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="G208" s="10" t="s">
+      <c r="G208" s="9" t="s">
         <v>384</v>
       </c>
       <c r="H208" s="1"/>
@@ -7325,19 +7315,19 @@
       <c r="A212" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B212" s="10" t="s">
+      <c r="B212" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="C212" s="10" t="s">
+      <c r="C212" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="D212" s="10" t="s">
+      <c r="D212" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="E212" s="10" t="s">
+      <c r="E212" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="F212" s="10" t="s">
+      <c r="F212" s="9" t="s">
         <v>396</v>
       </c>
       <c r="G212" s="1"/>
@@ -7368,7 +7358,7 @@
         <v>25</v>
       </c>
       <c r="G213" s="1"/>
-      <c r="H213" s="11"/>
+      <c r="H213" s="10"/>
       <c r="I213" s="1"/>
       <c r="J213" s="1"/>
       <c r="K213" s="1"/>
@@ -7942,7 +7932,7 @@
       <c r="L234" s="1"/>
       <c r="M234" s="1"/>
     </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
         <v>431</v>
       </c>
@@ -7969,7 +7959,7 @@
       <c r="L235" s="1"/>
       <c r="M235" s="1"/>
     </row>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
         <v>432</v>
       </c>
@@ -7996,7 +7986,7 @@
       <c r="L236" s="1"/>
       <c r="M236" s="1"/>
     </row>
-    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
         <v>433</v>
       </c>
@@ -8023,7 +8013,7 @@
       <c r="L237" s="1"/>
       <c r="M237" s="1"/>
     </row>
-    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
         <v>434</v>
       </c>
@@ -8050,7 +8040,7 @@
       <c r="L238" s="1"/>
       <c r="M238" s="1"/>
     </row>
-    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
         <v>435</v>
       </c>
@@ -8077,7 +8067,7 @@
       <c r="L239" s="1"/>
       <c r="M239" s="1"/>
     </row>
-    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
         <v>436</v>
       </c>
@@ -8104,7 +8094,7 @@
       <c r="L240" s="1"/>
       <c r="M240" s="1"/>
     </row>
-    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
         <v>437</v>
       </c>
@@ -8131,7 +8121,7 @@
       <c r="L241" s="1"/>
       <c r="M241" s="1"/>
     </row>
-    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
         <v>438</v>
       </c>
@@ -8158,7 +8148,7 @@
       <c r="L242" s="1"/>
       <c r="M242" s="1"/>
     </row>
-    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
         <v>439</v>
       </c>
@@ -8185,7 +8175,7 @@
       <c r="L243" s="1"/>
       <c r="M243" s="1"/>
     </row>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
         <v>440</v>
       </c>
@@ -8212,7 +8202,7 @@
       <c r="L244" s="1"/>
       <c r="M244" s="1"/>
     </row>
-    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
         <v>441</v>
       </c>
@@ -8239,7 +8229,7 @@
       <c r="L245" s="1"/>
       <c r="M245" s="1"/>
     </row>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
         <v>442</v>
       </c>
@@ -8266,7 +8256,7 @@
       <c r="L246" s="1"/>
       <c r="M246" s="1"/>
     </row>
-    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
         <v>443</v>
       </c>
@@ -8293,7 +8283,7 @@
       <c r="L247" s="1"/>
       <c r="M247" s="1"/>
     </row>
-    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
         <v>444</v>
       </c>
@@ -8320,7 +8310,7 @@
       <c r="L248" s="1"/>
       <c r="M248" s="1"/>
     </row>
-    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
         <v>445</v>
       </c>
@@ -8347,7 +8337,7 @@
       <c r="L249" s="1"/>
       <c r="M249" s="1"/>
     </row>
-    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
         <v>446</v>
       </c>
@@ -8374,7 +8364,7 @@
       <c r="L250" s="1"/>
       <c r="M250" s="1"/>
     </row>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
         <v>447</v>
       </c>
@@ -8401,7 +8391,7 @@
       <c r="L251" s="1"/>
       <c r="M251" s="1"/>
     </row>
-    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
         <v>448</v>
       </c>
@@ -8435,7 +8425,7 @@
       <c r="B253" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C253" s="10" t="s">
+      <c r="C253" s="9" t="s">
         <v>450</v>
       </c>
       <c r="D253" s="1" t="s">
@@ -8462,7 +8452,7 @@
       <c r="B254" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C254" s="10" t="s">
+      <c r="C254" s="9" t="s">
         <v>450</v>
       </c>
       <c r="D254" s="1" t="s">
@@ -8489,7 +8479,7 @@
       <c r="B255" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C255" s="10" t="s">
+      <c r="C255" s="9" t="s">
         <v>450</v>
       </c>
       <c r="D255" s="2" t="s">

</xml_diff>